<commit_message>
Temporary fix for non-display of tweets
</commit_message>
<xml_diff>
--- a/trail.xlsx
+++ b/trail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Negative tweets:</t>
   </si>
@@ -32,13 +32,100 @@
   </si>
   <si>
     <t>tweet</t>
+  </si>
+  <si>
+    <t>Sep 09 2017</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905906972393963520</t>
+  </si>
+  <si>
+    <t>#0daytoday #Apache Struts 2 REST Plugin XStream Remote Code Execution #Exploit #0day https://t.co/rwaxBrUvuC</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905906732098088966</t>
+  </si>
+  <si>
+    <t>#0daytoday #SourceTree Remote Code Execution #Exploit https://t.co/cGo5U8zYGm</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905878605128884225</t>
+  </si>
+  <si>
+    <t>#0daytoday #Gh0st Client - Buffer Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/ce22CcFpwa</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905878602645897217</t>
+  </si>
+  <si>
+    <t>#0daytoday #PlugX Controller Stack Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/jcciGj0kBX</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905750181722947584</t>
+  </si>
+  <si>
+    <t>#0daytoday #Apache #Struts 2.5 - Remote Code Execution #0day #Exploit https://t.co/NRIvcrWlEq</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905728881197408257</t>
+  </si>
+  <si>
+    <t>#0daytoday #WordPress Gym Management System Code Execution / Remote Cross Site Scripting Vulnerabil [#0day #Exploit] https://t.co/6BbjaqVOyR</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905513948224438272</t>
+  </si>
+  <si>
+    <t>#0daytoday #Tor - Linux Sandbox Breakout via X11 Exploit [remote #exploits #0day #Exploit] https://t.co/8bCWbuT4Uv</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905505647285813252</t>
+  </si>
+  <si>
+    <t>#0daytoday #Jungo DriverWizard WinDriver - Kernel Pool Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/jc9QMlrawK</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905355158887907328</t>
+  </si>
+  <si>
+    <t>#0daytoday #Samsung Internet Browser - SOP Bypass Exploit [remote #exploits #0day #Exploit] https://t.co/ka6tQuu1ZI</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/905079577915088897</t>
+  </si>
+  <si>
+    <t>#0daytoday #NEC EXPRESS CLUSTER clpwebmc Remote #Root #Exploit #0day https://t.co/4i3pB8Hwp8</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/904803563603406850</t>
+  </si>
+  <si>
+    <t>#0daytoday #RubyGems &amp;lt; 2.6.13 - Arbitrary File Overwrite #Exploit https://t.co/sM5XxS3Rxt</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/904743627418513408</t>
+  </si>
+  <si>
+    <t>#0daytoday #Wireless Repeater BE126 - Remote Code Execution Exploit [webapps #exploits #0day #Exploit] https://t.co/MJBKKmDAxw</t>
+  </si>
+  <si>
+    <t>Aug 08 2017</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/902990838938058752</t>
+  </si>
+  <si>
+    <t>#0daytoday #Joomla Joomanager 2.0.0 Component - Arbitrary File Download Vulnerability [#0day #Exploit] https://t.co/OJCfpL4p9I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,6 +137,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,9 +170,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E3"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -400,7 +496,243 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>-0.1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>-0.1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>-0.1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>-0.1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>-0.1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>-0.05</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>-0.1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>-0.1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>-0.1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>-0.1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>-0.1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>-0.1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>-0.1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
+    <hyperlink ref="D7" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix saved_tweets list index range error
</commit_message>
<xml_diff>
--- a/trail.xlsx
+++ b/trail.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="44">
   <si>
     <t>Negative tweets:</t>
   </si>
@@ -40,85 +40,112 @@
     <t>negative</t>
   </si>
   <si>
-    <t>https://twitter.com/statuses/905906972393963520</t>
-  </si>
-  <si>
-    <t>#0daytoday #Apache Struts 2 REST Plugin XStream Remote Code Execution #Exploit #0day https://t.co/rwaxBrUvuC</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905906732098088966</t>
-  </si>
-  <si>
-    <t>#0daytoday #SourceTree Remote Code Execution #Exploit https://t.co/cGo5U8zYGm</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905878605128884225</t>
-  </si>
-  <si>
-    <t>#0daytoday #Gh0st Client - Buffer Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/ce22CcFpwa</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905878602645897217</t>
-  </si>
-  <si>
-    <t>#0daytoday #PlugX Controller Stack Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/jcciGj0kBX</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905750181722947584</t>
-  </si>
-  <si>
-    <t>#0daytoday #Apache #Struts 2.5 - Remote Code Execution #0day #Exploit https://t.co/NRIvcrWlEq</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905728881197408257</t>
-  </si>
-  <si>
-    <t>#0daytoday #WordPress Gym Management System Code Execution / Remote Cross Site Scripting Vulnerabil [#0day #Exploit] https://t.co/6BbjaqVOyR</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905513948224438272</t>
-  </si>
-  <si>
-    <t>#0daytoday #Tor - Linux Sandbox Breakout via X11 Exploit [remote #exploits #0day #Exploit] https://t.co/8bCWbuT4Uv</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905505647285813252</t>
-  </si>
-  <si>
-    <t>#0daytoday #Jungo DriverWizard WinDriver - Kernel Pool Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/jc9QMlrawK</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905355158887907328</t>
-  </si>
-  <si>
-    <t>#0daytoday #Samsung Internet Browser - SOP Bypass Exploit [remote #exploits #0day #Exploit] https://t.co/ka6tQuu1ZI</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/905079577915088897</t>
-  </si>
-  <si>
-    <t>#0daytoday #NEC EXPRESS CLUSTER clpwebmc Remote #Root #Exploit #0day https://t.co/4i3pB8Hwp8</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/904803563603406850</t>
-  </si>
-  <si>
-    <t>#0daytoday #RubyGems &amp;lt; 2.6.13 - Arbitrary File Overwrite #Exploit https://t.co/sM5XxS3Rxt</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/904743627418513408</t>
-  </si>
-  <si>
-    <t>#0daytoday #Wireless Repeater BE126 - Remote Code Execution Exploit [webapps #exploits #0day #Exploit] https://t.co/MJBKKmDAxw</t>
-  </si>
-  <si>
-    <t>Aug 08 2017</t>
-  </si>
-  <si>
-    <t>https://twitter.com/statuses/902990838938058752</t>
-  </si>
-  <si>
-    <t>#0daytoday #Joomla Joomanager 2.0.0 Component - Arbitrary File Download Vulnerability [#0day #Exploit] https://t.co/OJCfpL4p9I</t>
+    <t>https://twitter.com/statuses/910212924504866817</t>
+  </si>
+  <si>
+    <t>#0daytoday #Tecnovision DLX Spot - Arbitrary File Upload Vulnerability [remote #exploits #Vulnerability #0day… https://t.co/tj8JlLp2NM</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/910212922143522816</t>
+  </si>
+  <si>
+    <t>#0daytoday #Tecnovision DLX Spot - Authentication Bypass Vulnerability [remote #exploits #Vulnerability #0day… https://t.co/wpMvHxrNGV</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/910212919547240448</t>
+  </si>
+  <si>
+    <t>#0daytoday #Tecnovision DLX Spot - SSH Backdoor Vulnerability CVE-2017-12928 [remote #exploits #Vulnerability #0day… https://t.co/k1z5DvTXx3</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/910204857511903232</t>
+  </si>
+  <si>
+    <t>#0daytoday #HPE &amp;amp;lt; 7.2 - Java Deserialization Exploit CVE-2016-4372 [remote #exploits #0day #Exploit] https://t.co/HzChSlUqJA</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/909700296158339072</t>
+  </si>
+  <si>
+    <t>#0daytoday #Netdecision 5.8.2 - Local Privilege Escalation Exploit CVE-2017-14311 [remote #exploits #0day #Exploit] https://t.co/hBu3SRhWx5</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/909526400612188160</t>
+  </si>
+  <si>
+    <t>#0daytoday #EMC Data Protection Advisor Hardcoded Password Vulnerability [remote #exploits #Vulnerability #0day… https://t.co/cKPXhkYoxS</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908810169148157953</t>
+  </si>
+  <si>
+    <t>#0daytoday #Astaro Security Gateway 7 Remote Code Execution #Exploit https://t.co/GoZqzFZIkl</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908809924876099587</t>
+  </si>
+  <si>
+    <t>#0daytoday #DLink DIR8xx Remote Root Code Execution #Exploit https://t.co/B98M14ZcxE</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908649382400073728</t>
+  </si>
+  <si>
+    <t>#0daytoday #VLC Media Player iOS App 2.7.8 File Disclosure Vulnerability [remote #exploits #Vulnerability #0day… https://t.co/et1wT2KvKZ</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908649380026097666</t>
+  </si>
+  <si>
+    <t>#0daytoday #VIPA Automation WinPLC7 5.0.45.5921 Buffer Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/SBIYWWRYIn</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908649377253662724</t>
+  </si>
+  <si>
+    <t>#0daytoday #Disk Pulse Server 2.2.34 Buffer Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/BujSgn4Tn3</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908649374812479488</t>
+  </si>
+  <si>
+    <t>#0daytoday #haneWIN DNS Server 1.5.3 Buffer Overflow Exploit [remote #exploits #0day #Exploit] https://t.co/YAFn3NKaW5</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908649372778246144</t>
+  </si>
+  <si>
+    <t>#0daytoday #KingScada AlarmServer 3.1.2.13 Buffer Overflow Exploit CVE-2014-0787 [remote #exploits #0day #Exploit] https://t.co/w6UILqQNJo</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908083799296299008</t>
+  </si>
+  <si>
+    <t>#0daytoday #EMC CMCNE Inmservlets.war FileUploadController 11.2.1 - Remote Code Execution #Exploit https://t.co/qB4nS4Wrxe</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908083683684470784</t>
+  </si>
+  <si>
+    <t>#0daytoday #EMC CMCNE 11.2.1 - FileUploadController Remote Code Execution #Exploit https://t.co/0Ot4rUrdbL</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908083588989628416</t>
+  </si>
+  <si>
+    <t>#0daytoday #Dameware Mini Remote Control 4.0 - Username Stack Buffer Overflow #Exploit https://t.co/fN7utYLvTi</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908083451194167296</t>
+  </si>
+  <si>
+    <t>#0daytoday #Cloudview NMS &amp;lt; 2.00b - Arbitrary File Upload #Exploit https://t.co/ItHdb4XWJD</t>
+  </si>
+  <si>
+    <t>https://twitter.com/statuses/908035000179859456</t>
+  </si>
+  <si>
+    <t>#0daytoday #Microsoft #Windows .NET #Framework - Remote Code Execution #0day #Exploit https://t.co/lSpKziNdZs</t>
   </si>
 </sst>
 </file>
@@ -468,7 +495,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E16"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -572,7 +599,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>-0.1</v>
+        <v>-0.05</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>16</v>
@@ -589,7 +616,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
@@ -702,19 +729,104 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>-0.1</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>-0.1</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" t="s">
         <v>33</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>-0.1</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>34</v>
+      </c>
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>-0.1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>-0.1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>-0.1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>-0.1</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -732,6 +844,11 @@
     <hyperlink ref="D14" r:id="rId11"/>
     <hyperlink ref="D15" r:id="rId12"/>
     <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>